<commit_message>
+ chỉnh lại số thẻ bị sai
</commit_message>
<xml_diff>
--- a/Bao Cao Lien Tuc/Chuan_Bi_Du_Lieu_Test.xlsx
+++ b/Bao Cao Lien Tuc/Chuan_Bi_Du_Lieu_Test.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="62">
   <si>
     <t xml:space="preserve">Chức năng </t>
   </si>
@@ -150,6 +150,57 @@
   </si>
   <si>
     <t>vanchuyen</t>
+  </si>
+  <si>
+    <t>Số tài khoản:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Chuyển tiền _ Cùng Môi Giới</t>
+  </si>
+  <si>
+    <t>Chuyển Tiền _Khác Môi Giới</t>
+  </si>
+  <si>
+    <t>4024007182425917</t>
+  </si>
+  <si>
+    <t>4024007186826466</t>
+  </si>
+  <si>
+    <t>4024007186826862</t>
+  </si>
+  <si>
+    <t>4024007187096481</t>
+  </si>
+  <si>
+    <t>4024007187426415</t>
+  </si>
+  <si>
+    <t>340426820759153</t>
+  </si>
+  <si>
+    <t>4024007186815758</t>
+  </si>
+  <si>
+    <t>4024007186825765</t>
+  </si>
+  <si>
+    <t>340429813757143</t>
+  </si>
+  <si>
+    <t>5119358642641939</t>
+  </si>
+  <si>
+    <t>5119358702641035</t>
+  </si>
+  <si>
+    <t>5119358742641037</t>
+  </si>
+  <si>
+    <t>5119359792646041</t>
   </si>
 </sst>
 </file>
@@ -169,14 +220,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -191,7 +241,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -214,69 +264,154 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="168" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -580,542 +715,944 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="28.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="9.140625" style="10"/>
+    <col min="2" max="2" width="31.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24" style="10" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="32" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="A7" s="27">
         <v>1</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="33" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="3"/>
+      <c r="D7" s="33"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="A9" s="27">
         <v>2</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="7" t="s">
+      <c r="C9" s="27"/>
+      <c r="D9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="3"/>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="8">
-        <v>4024007186826460</v>
-      </c>
-      <c r="E10" s="8">
-        <v>4024007186826860</v>
-      </c>
-      <c r="F10" s="8">
-        <v>4024007187096480</v>
-      </c>
-      <c r="G10" s="8">
-        <v>4024007187426410</v>
+      <c r="D10" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="34" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="3"/>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="6">
-        <v>123456</v>
-      </c>
-      <c r="E11" s="6">
-        <v>123456</v>
-      </c>
-      <c r="F11" s="6">
-        <v>123456</v>
-      </c>
-      <c r="G11" s="6">
+      <c r="D11" s="27">
+        <v>123456</v>
+      </c>
+      <c r="E11" s="27">
+        <v>123456</v>
+      </c>
+      <c r="F11" s="27">
+        <v>123456</v>
+      </c>
+      <c r="G11" s="27">
         <v>123456</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="3"/>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="27">
         <v>33857</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="G12" s="27" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="3"/>
-      <c r="D13" s="10"/>
-    </row>
-    <row r="14" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
+      <c r="D13" s="35"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="27">
         <v>3</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="7" t="s">
+      <c r="C14" s="27"/>
+      <c r="D14" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F14" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="G14" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H14" s="7" t="s">
+      <c r="H14" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="11" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="C15" s="12" t="s">
+    <row r="15" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G15" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="H15" s="36" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="3"/>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="6">
-        <v>12345678</v>
-      </c>
-      <c r="E16" s="6">
-        <v>12345678</v>
-      </c>
-      <c r="F16" s="6">
-        <v>12345678</v>
-      </c>
-      <c r="G16" s="6">
-        <v>12345678</v>
-      </c>
-      <c r="H16" s="6">
+      <c r="D16" s="27">
+        <v>12345678</v>
+      </c>
+      <c r="E16" s="27">
+        <v>12345678</v>
+      </c>
+      <c r="F16" s="27">
+        <v>12345678</v>
+      </c>
+      <c r="G16" s="27">
+        <v>12345678</v>
+      </c>
+      <c r="H16" s="27">
         <v>12345678</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
+      <c r="A18" s="27">
         <v>4</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C19" s="6"/>
-      <c r="D19" s="7" t="s">
+      <c r="C18" s="27"/>
+      <c r="D18" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E18" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="F18" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G19" s="7" t="s">
+      <c r="G18" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H19" s="7" t="s">
+      <c r="H18" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F20" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="G20" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="H20" s="36" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="6">
-        <v>12345678</v>
-      </c>
-      <c r="E21" s="6">
-        <v>12345678</v>
-      </c>
-      <c r="F21" s="6">
-        <v>12345678</v>
-      </c>
-      <c r="G21" s="6">
-        <v>12345678</v>
-      </c>
-      <c r="H21" s="6">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="14" t="s">
+      <c r="D21" s="27">
+        <v>12345678</v>
+      </c>
+      <c r="E21" s="27">
+        <v>12345678</v>
+      </c>
+      <c r="F21" s="27">
+        <v>12345678</v>
+      </c>
+      <c r="G21" s="27">
+        <v>12345678</v>
+      </c>
+      <c r="H21" s="27">
+        <v>12345678</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C22" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="8">
-        <v>340426820759153</v>
-      </c>
-      <c r="E22" s="8">
-        <v>4024007186815750</v>
-      </c>
-      <c r="F22" s="8">
-        <v>4024007186825760</v>
-      </c>
-      <c r="G22" s="8">
-        <v>340429813757143</v>
-      </c>
-      <c r="H22" s="8">
-        <v>4024007182425910</v>
+      <c r="D22" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="F22" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="G22" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="H22" s="34" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D23" s="6">
-        <v>123456</v>
-      </c>
-      <c r="E23" s="6">
-        <v>123456</v>
-      </c>
-      <c r="F23" s="6">
-        <v>123456</v>
-      </c>
-      <c r="G23" s="6">
-        <v>123456</v>
-      </c>
-      <c r="H23" s="6">
-        <v>123456</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="17" t="s">
+      <c r="D23" s="27">
+        <v>123456</v>
+      </c>
+      <c r="E23" s="27">
+        <v>123456</v>
+      </c>
+      <c r="F23" s="27">
+        <v>123456</v>
+      </c>
+      <c r="G23" s="27">
+        <v>123456</v>
+      </c>
+      <c r="H23" s="27">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C24" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="D24" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="E24" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="F24" s="9" t="s">
+      <c r="F24" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="G24" s="9" t="s">
+      <c r="G24" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="H24" s="9" t="s">
+      <c r="H24" s="27" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="7" t="s">
+      <c r="A27" s="27">
+        <v>5</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G27" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="H27" s="7" t="s">
-        <v>29</v>
-      </c>
+      <c r="C27" s="37"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="38"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D29" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="F29" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="G29" s="1" t="s">
+      <c r="G29" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="H29" s="36" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D30" s="6">
-        <v>12345678</v>
-      </c>
-      <c r="E30" s="6">
-        <v>12345678</v>
-      </c>
-      <c r="F30" s="6">
-        <v>12345678</v>
-      </c>
-      <c r="G30" s="6">
-        <v>12345678</v>
-      </c>
-      <c r="H30" s="6">
+      <c r="D30" s="27">
+        <v>12345678</v>
+      </c>
+      <c r="E30" s="27">
+        <v>12345678</v>
+      </c>
+      <c r="F30" s="27">
+        <v>12345678</v>
+      </c>
+      <c r="G30" s="27">
+        <v>12345678</v>
+      </c>
+      <c r="H30" s="27">
         <v>12345678</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="C31" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="D31" s="8">
-        <v>340426820759153</v>
-      </c>
-      <c r="E31" s="8">
-        <v>4024007186815750</v>
-      </c>
-      <c r="F31" s="8">
-        <v>4024007186825760</v>
-      </c>
-      <c r="G31" s="8">
-        <v>340429813757143</v>
-      </c>
-      <c r="H31" s="8">
-        <v>4024007182425910</v>
+      <c r="D31" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="E31" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="F31" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="G31" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="H31" s="34" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D32" s="6">
-        <v>123456</v>
-      </c>
-      <c r="E32" s="6">
-        <v>123456</v>
-      </c>
-      <c r="F32" s="6">
-        <v>123456</v>
-      </c>
-      <c r="G32" s="6">
-        <v>123456</v>
-      </c>
-      <c r="H32" s="6">
-        <v>123456</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C33" s="17" t="s">
+      <c r="D32" s="27">
+        <v>123456</v>
+      </c>
+      <c r="E32" s="27">
+        <v>123456</v>
+      </c>
+      <c r="F32" s="27">
+        <v>123456</v>
+      </c>
+      <c r="G32" s="27">
+        <v>123456</v>
+      </c>
+      <c r="H32" s="27">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C33" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D33" s="9" t="s">
+      <c r="D33" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="E33" s="9" t="s">
+      <c r="E33" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="F33" s="9" t="s">
+      <c r="F33" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="G33" s="9" t="s">
+      <c r="G33" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="H33" s="9" t="s">
+      <c r="H33" s="27" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C36" s="5" t="s">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C36" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D36" s="19" t="s">
+      <c r="D36" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="E36" s="19" t="s">
+      <c r="E36" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="F36" s="19" t="s">
+      <c r="F36" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="G36" s="1" t="s">
+      <c r="G36" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="H36" s="1"/>
-    </row>
-    <row r="37" spans="1:8" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="13"/>
-      <c r="B37" s="20" t="s">
+      <c r="H36" s="36"/>
+    </row>
+    <row r="37" spans="2:8" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C37" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D37" s="19">
-        <v>123456</v>
-      </c>
-      <c r="E37" s="19">
-        <v>123456</v>
-      </c>
-      <c r="F37" s="19">
-        <v>123456</v>
-      </c>
-      <c r="G37" s="19">
-        <v>123456</v>
-      </c>
-      <c r="H37" s="6"/>
-    </row>
-    <row r="38" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C38" s="14" t="s">
+      <c r="D37" s="36">
+        <v>123456</v>
+      </c>
+      <c r="E37" s="36">
+        <v>123456</v>
+      </c>
+      <c r="F37" s="36">
+        <v>123456</v>
+      </c>
+      <c r="G37" s="36">
+        <v>123456</v>
+      </c>
+      <c r="H37" s="27"/>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C38" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="D38" s="21">
-        <v>5119358642641930</v>
-      </c>
-      <c r="E38" s="21">
-        <v>5119358702641030</v>
-      </c>
-      <c r="F38" s="21">
-        <v>5119358742641030</v>
-      </c>
-      <c r="G38" s="21">
-        <v>5119359792646040</v>
-      </c>
-      <c r="H38" s="8"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C39" s="5" t="s">
+      <c r="D38" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="E38" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="F38" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="G38" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="H38" s="39"/>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C39" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D39" s="6">
-        <v>123456</v>
-      </c>
-      <c r="E39" s="6">
-        <v>123456</v>
-      </c>
-      <c r="F39" s="6">
-        <v>123456</v>
-      </c>
-      <c r="G39" s="6">
-        <v>123456</v>
-      </c>
-      <c r="H39" s="6"/>
+      <c r="D39" s="27">
+        <v>123456</v>
+      </c>
+      <c r="E39" s="27">
+        <v>123456</v>
+      </c>
+      <c r="F39" s="27">
+        <v>123456</v>
+      </c>
+      <c r="G39" s="27">
+        <v>123456</v>
+      </c>
+      <c r="H39" s="27"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C7:D7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A6:H50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:F21"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="17.42578125" customWidth="1"/>
-    <col min="5" max="5" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="9"/>
+    <col min="2" max="2" width="31.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="6"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="8"/>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>2</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C11" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="11">
+        <v>12345678</v>
+      </c>
+      <c r="E11" s="11">
+        <v>12345678</v>
+      </c>
+      <c r="F11" s="11">
+        <v>12345678</v>
+      </c>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C12" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="14">
+        <v>358984</v>
+      </c>
+      <c r="E12" s="14">
+        <v>948676</v>
+      </c>
+      <c r="F12" s="14">
+        <v>584739</v>
+      </c>
+      <c r="G12" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12" s="22"/>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D13" s="15"/>
+      <c r="G13" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="9"/>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
+        <v>4</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="11"/>
+      <c r="D18" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C20" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C21" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="11">
+        <v>12345678</v>
+      </c>
+      <c r="E21" s="11">
+        <v>12345678</v>
+      </c>
+      <c r="F21" s="11">
+        <v>12345678</v>
+      </c>
+      <c r="G21" s="11"/>
+    </row>
+    <row r="22" spans="1:8" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="16"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="13">
+        <v>4024007186815750</v>
+      </c>
+      <c r="E22" s="13">
+        <v>4024007186825760</v>
+      </c>
+      <c r="F22" s="13">
+        <v>4024007182425910</v>
+      </c>
+      <c r="G22" s="13"/>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C23" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="11">
+        <v>123456</v>
+      </c>
+      <c r="E23" s="11">
+        <v>123456</v>
+      </c>
+      <c r="F23" s="11">
+        <v>123456</v>
+      </c>
+      <c r="G23" s="11"/>
+    </row>
+    <row r="24" spans="1:8" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="10"/>
+      <c r="C24" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G24" s="14"/>
+    </row>
+    <row r="25" spans="1:8" s="30" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="28"/>
+      <c r="B25" s="29"/>
+      <c r="F25" s="30">
+        <v>4024007182425910</v>
+      </c>
+      <c r="G25" s="30">
+        <v>4024007182425910</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G26" s="31" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
+        <v>5</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="22"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
+    </row>
+    <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C29" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C30" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" s="11">
+        <v>12345678</v>
+      </c>
+      <c r="E30" s="11">
+        <v>12345678</v>
+      </c>
+      <c r="F30" s="11">
+        <v>12345678</v>
+      </c>
+      <c r="G30" s="11"/>
+    </row>
+    <row r="31" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B31" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" s="13">
+        <v>4024007186815750</v>
+      </c>
+      <c r="E31" s="13">
+        <v>4024007186825760</v>
+      </c>
+      <c r="F31" s="13">
+        <v>4024007182425910</v>
+      </c>
+      <c r="G31" s="13"/>
+    </row>
+    <row r="32" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C32" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" s="11">
+        <v>123456</v>
+      </c>
+      <c r="E32" s="11">
+        <v>123456</v>
+      </c>
+      <c r="F32" s="11">
+        <v>123456</v>
+      </c>
+      <c r="G32" s="11"/>
+    </row>
+    <row r="33" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C33" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="F33" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G33" s="14"/>
+    </row>
+    <row r="36" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C36" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H36" s="1"/>
+    </row>
+    <row r="37" spans="1:8" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="16"/>
+      <c r="B37" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" s="1">
+        <v>123456</v>
+      </c>
+      <c r="E37" s="1">
+        <v>123456</v>
+      </c>
+      <c r="F37" s="1">
+        <v>123456</v>
+      </c>
+      <c r="G37" s="1">
+        <v>123456</v>
+      </c>
+      <c r="H37" s="11"/>
+    </row>
+    <row r="38" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C38" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" s="2">
+        <v>5119358642641930</v>
+      </c>
+      <c r="E38" s="2">
+        <v>5119358702641030</v>
+      </c>
+      <c r="F38" s="2">
+        <v>5119358742641030</v>
+      </c>
+      <c r="G38" s="2">
+        <v>5119359792646040</v>
+      </c>
+      <c r="H38" s="13"/>
+    </row>
+    <row r="39" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C39" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" s="11">
+        <v>123456</v>
+      </c>
+      <c r="E39" s="11">
+        <v>123456</v>
+      </c>
+      <c r="F39" s="11">
+        <v>123456</v>
+      </c>
+      <c r="G39" s="11">
+        <v>123456</v>
+      </c>
+      <c r="H39" s="11"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="9">
+        <v>6</v>
+      </c>
+      <c r="B42" s="27" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C7:D7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>